<commit_message>
long sword 엑셀 저장 및 db 등록
</commit_message>
<xml_diff>
--- a/app/weapon_data.xlsx
+++ b/app/weapon_data.xlsx
@@ -4,11 +4,11 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="30" windowWidth="25755" windowHeight="11595" tabRatio="590" activeTab="0"/>
+    <workbookView xWindow="360" yWindow="30" windowWidth="25755" windowHeight="11595" tabRatio="580" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Great_Sword" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Long_Sword" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="478" uniqueCount="478">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="565" uniqueCount="565">
   <si>
     <t>용골대검 I</t>
   </si>
@@ -1443,6 +1443,267 @@
   </si>
   <si>
     <t>첨룡골*10</t>
+  </si>
+  <si>
+    <t>철도 I</t>
+  </si>
+  <si>
+    <t>철도 II</t>
+  </si>
+  <si>
+    <t>철도 III</t>
+  </si>
+  <si>
+    <t>철도 [계] I</t>
+  </si>
+  <si>
+    <t>철도 [계] II</t>
+  </si>
+  <si>
+    <t>철도 [계] III</t>
+  </si>
+  <si>
+    <t>철도 [신락] I</t>
+  </si>
+  <si>
+    <t>철도 [신락] II</t>
+  </si>
+  <si>
+    <t>네르갈리베</t>
+  </si>
+  <si>
+    <t>90(대)</t>
+  </si>
+  <si>
+    <t>멸절의일도</t>
+  </si>
+  <si>
+    <t>120(대)</t>
+  </si>
+  <si>
+    <t>현도 [요] I</t>
+  </si>
+  <si>
+    <t>현도 [요] II</t>
+  </si>
+  <si>
+    <t>현혹도 [섬] I</t>
+  </si>
+  <si>
+    <t>현혹도 [섬] II</t>
+  </si>
+  <si>
+    <t>현혹도 [섬] III</t>
+  </si>
+  <si>
+    <t>알리샤 I</t>
+  </si>
+  <si>
+    <t>알리샤 II</t>
+  </si>
+  <si>
+    <t>알리샤 III</t>
+  </si>
+  <si>
+    <t>알다자주 I</t>
+  </si>
+  <si>
+    <t>알다자주 II</t>
+  </si>
+  <si>
+    <t>알다자주 III</t>
+  </si>
+  <si>
+    <t>브라스리지 I</t>
+  </si>
+  <si>
+    <t>브라스리지 II</t>
+  </si>
+  <si>
+    <t>31-</t>
+  </si>
+  <si>
+    <t>비룡도 [청엽]</t>
+  </si>
+  <si>
+    <t>비룡도 [익]</t>
+  </si>
+  <si>
+    <t>비룡도 [규]</t>
+  </si>
+  <si>
+    <t>비룡도 [홍엽]</t>
+  </si>
+  <si>
+    <t>비룡도 [주]</t>
+  </si>
+  <si>
+    <t>비룡도 [창]</t>
+  </si>
+  <si>
+    <t>비룡도 [감염]</t>
+  </si>
+  <si>
+    <t>본쇼텔 I</t>
+  </si>
+  <si>
+    <t>본쇼텔 II</t>
+  </si>
+  <si>
+    <t>본쇼텔 III</t>
+  </si>
+  <si>
+    <t>하드본쇼텔 I</t>
+  </si>
+  <si>
+    <t>하드본쇼텔 II</t>
+  </si>
+  <si>
+    <t>하드본쇼텔 III</t>
+  </si>
+  <si>
+    <t>본리퍼 I</t>
+  </si>
+  <si>
+    <t>본리퍼 II</t>
+  </si>
+  <si>
+    <t>폭린의대도</t>
+  </si>
+  <si>
+    <t>폭린도바젤바르가</t>
+  </si>
+  <si>
+    <t>블레이즈쇼텔 I</t>
+  </si>
+  <si>
+    <t>블레이즈쇼텔 II</t>
+  </si>
+  <si>
+    <t>쟈나프시미터 I</t>
+  </si>
+  <si>
+    <t>쟈나프시미터 II</t>
+  </si>
+  <si>
+    <t>쟈나프시미터 III</t>
+  </si>
+  <si>
+    <t>슈람쇼텔 I</t>
+  </si>
+  <si>
+    <t>슈람쇼텔 II</t>
+  </si>
+  <si>
+    <t>슈람쇼텔 III</t>
+  </si>
+  <si>
+    <t>디프테루스 I</t>
+  </si>
+  <si>
+    <t>디프테루스 II</t>
+  </si>
+  <si>
+    <t>디프테루스 III</t>
+  </si>
+  <si>
+    <t>하자크그로서 I</t>
+  </si>
+  <si>
+    <t>210(중)</t>
+  </si>
+  <si>
+    <t>하자크그로서 II</t>
+  </si>
+  <si>
+    <t>270(중)</t>
+  </si>
+  <si>
+    <t>펄서쇼텔 I</t>
+  </si>
+  <si>
+    <t>펄서쇼텔 II</t>
+  </si>
+  <si>
+    <t>펄서쇼텔 III</t>
+  </si>
+  <si>
+    <t>카가치의송곳니 I</t>
+  </si>
+  <si>
+    <t>카가치의송곳니 II</t>
+  </si>
+  <si>
+    <t>카가치의송곳니 III</t>
+  </si>
+  <si>
+    <t>그레이스쇼텔 I</t>
+  </si>
+  <si>
+    <t>그레이스쇼텔 II</t>
+  </si>
+  <si>
+    <t>스틸러</t>
+  </si>
+  <si>
+    <t>레이스틸러</t>
+  </si>
+  <si>
+    <t>다크쇼텔 I</t>
+  </si>
+  <si>
+    <t>다크쇼텔 II</t>
+  </si>
+  <si>
+    <t>다크시미터 I</t>
+  </si>
+  <si>
+    <t>다크시미터 II</t>
+  </si>
+  <si>
+    <t>다크시미터 III</t>
+  </si>
+  <si>
+    <t>용골도 I</t>
+  </si>
+  <si>
+    <t>용골도 II</t>
+  </si>
+  <si>
+    <t>용골도 III</t>
+  </si>
+  <si>
+    <t>마그다-파클타스 I</t>
+  </si>
+  <si>
+    <t>마그다-파클타스 II</t>
+  </si>
+  <si>
+    <t>흑강의태도 I</t>
+  </si>
+  <si>
+    <t>흑강의태도 II</t>
+  </si>
+  <si>
+    <t>150(소)</t>
+  </si>
+  <si>
+    <t>제왕도</t>
+  </si>
+  <si>
+    <t>제왕도 [양염]</t>
+  </si>
+  <si>
+    <t>제노사이퍼</t>
+  </si>
+  <si>
+    <t>180(소)</t>
+  </si>
+  <si>
+    <t>천하무쌍도</t>
+  </si>
+  <si>
+    <t>천상천하무쌍도</t>
   </si>
 </sst>
 </file>
@@ -1454,7 +1715,7 @@
     <numFmt numFmtId="65" formatCode="0_);\(0\)"/>
     <numFmt numFmtId="66" formatCode="General"/>
   </numFmts>
-  <fonts count="25">
+  <fonts count="27">
     <font>
       <sz val="11.0"/>
       <name val="맑은 고딕"/>
@@ -1589,10 +1850,20 @@
     <font>
       <sz val="11.0"/>
       <name val="맑은 고딕"/>
+      <color theme="1"/>
+    </font>
+    <font>
+      <sz val="11.0"/>
+      <name val="맑은 고딕"/>
+      <color theme="1"/>
+    </font>
+    <font>
+      <sz val="11.0"/>
+      <name val="맑은 고딕"/>
       <color rgb="FF000000"/>
     </font>
   </fonts>
-  <fills count="40">
+  <fills count="41">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1829,16 +2100,20 @@
         <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor theme="0"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="35">
+  <borders count="38">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal style="none">
-        <color rgb="FF000000"/>
-      </diagonal>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -1853,25 +2128,33 @@
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
       </bottom>
-      <diagonal/>
+      <diagonal style="none">
+        <color rgb="FF000000"/>
+      </diagonal>
     </border>
     <border>
       <bottom style="thick">
         <color theme="4"/>
       </bottom>
-      <diagonal/>
+      <diagonal style="none">
+        <color rgb="FF000000"/>
+      </diagonal>
     </border>
     <border>
       <bottom style="thick">
         <color rgb="FFACCCEA"/>
       </bottom>
-      <diagonal/>
+      <diagonal style="none">
+        <color rgb="FF000000"/>
+      </diagonal>
     </border>
     <border>
       <bottom style="medium">
         <color theme="4" tint="0.399980"/>
       </bottom>
-      <diagonal/>
+      <diagonal style="none">
+        <color rgb="FF000000"/>
+      </diagonal>
     </border>
     <border>
       <left style="thin">
@@ -1886,7 +2169,9 @@
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
       </bottom>
-      <diagonal/>
+      <diagonal style="none">
+        <color rgb="FF000000"/>
+      </diagonal>
     </border>
     <border>
       <left style="thin">
@@ -1901,7 +2186,9 @@
       <bottom style="thin">
         <color rgb="FF3F3F3F"/>
       </bottom>
-      <diagonal/>
+      <diagonal style="none">
+        <color rgb="FF000000"/>
+      </diagonal>
     </border>
     <border>
       <left style="double">
@@ -1916,13 +2203,17 @@
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
       </bottom>
-      <diagonal/>
+      <diagonal style="none">
+        <color rgb="FF000000"/>
+      </diagonal>
     </border>
     <border>
       <bottom style="double">
         <color rgb="FFFF8001"/>
       </bottom>
-      <diagonal/>
+      <diagonal style="none">
+        <color rgb="FF000000"/>
+      </diagonal>
     </border>
     <border>
       <top style="thin">
@@ -1930,6 +2221,23 @@
       </top>
       <bottom style="double">
         <color theme="4"/>
+      </bottom>
+      <diagonal style="none">
+        <color rgb="FF000000"/>
+      </diagonal>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1945,6 +2253,339 @@
       </top>
       <bottom style="thin">
         <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="1"/>
+      </left>
+      <right style="thin">
+        <color theme="1"/>
+      </right>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="1"/>
+      </left>
+      <right style="thin">
+        <color theme="1"/>
+      </right>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="1"/>
+      </left>
+      <right style="thin">
+        <color theme="1"/>
+      </right>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom style="thin">
+        <color theme="1"/>
       </bottom>
       <diagonal style="none">
         <color rgb="FF000000"/>
@@ -1967,355 +2608,6 @@
         <color rgb="FF000000"/>
       </diagonal>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal style="none">
-        <color rgb="FF000000"/>
-      </diagonal>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal style="none">
-        <color rgb="FF000000"/>
-      </diagonal>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal style="none">
-        <color rgb="FF000000"/>
-      </diagonal>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal style="none">
-        <color rgb="FF000000"/>
-      </diagonal>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal style="none">
-        <color rgb="FF000000"/>
-      </diagonal>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal style="none">
-        <color rgb="FF000000"/>
-      </diagonal>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal style="none">
-        <color rgb="FF000000"/>
-      </diagonal>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal style="none">
-        <color rgb="FF000000"/>
-      </diagonal>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal style="none">
-        <color rgb="FF000000"/>
-      </diagonal>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal style="none">
-        <color rgb="FF000000"/>
-      </diagonal>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal style="none">
-        <color rgb="FF000000"/>
-      </diagonal>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal style="none">
-        <color rgb="FF000000"/>
-      </diagonal>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal style="none">
-        <color rgb="FF000000"/>
-      </diagonal>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal style="none">
-        <color rgb="FF000000"/>
-      </diagonal>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal style="none">
-        <color rgb="FF000000"/>
-      </diagonal>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom/>
-      <diagonal style="none">
-        <color rgb="FF000000"/>
-      </diagonal>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom/>
-      <diagonal style="none">
-        <color rgb="FF000000"/>
-      </diagonal>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal style="none">
-        <color rgb="FF000000"/>
-      </diagonal>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal style="none">
-        <color rgb="FF000000"/>
-      </diagonal>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal style="none">
-        <color rgb="FF000000"/>
-      </diagonal>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal style="none">
-        <color rgb="FF000000"/>
-      </diagonal>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal style="none">
-        <color rgb="FF000000"/>
-      </diagonal>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="1"/>
-      </left>
-      <right style="thin">
-        <color theme="1"/>
-      </right>
-      <top style="thin">
-        <color theme="1"/>
-      </top>
-      <bottom style="thin">
-        <color theme="1"/>
-      </bottom>
-      <diagonal style="none">
-        <color rgb="FF000000"/>
-      </diagonal>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -2466,7 +2758,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="125">
+  <cellXfs count="135">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -2836,7 +3128,37 @@
     <xf numFmtId="0" fontId="20" fillId="39" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0">
+    <xf numFmtId="0" fontId="24" fillId="40" borderId="10" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="40" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="40" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="40" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="40" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="40" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="40" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="65" fontId="24" fillId="40" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="37" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="66" fontId="0" fillId="33" borderId="34" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -3163,8 +3485,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AE91"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O25" sqref="O25"/>
+    <sheetView topLeftCell="A6" tabSelected="1" workbookViewId="0">
+      <selection activeCell="J90" sqref="J90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.500000"/>
@@ -3278,7 +3600,7 @@
       <c r="G2" s="100"/>
       <c r="H2" s="100"/>
       <c r="I2" s="105"/>
-      <c r="J2" s="124">
+      <c r="J2" s="134">
         <v>0</v>
       </c>
       <c r="K2" s="100"/>
@@ -3314,7 +3636,7 @@
       <c r="G3" s="100"/>
       <c r="H3" s="100"/>
       <c r="I3" s="105"/>
-      <c r="J3" s="124">
+      <c r="J3" s="134">
         <v>0</v>
       </c>
       <c r="K3" s="100"/>
@@ -3353,7 +3675,7 @@
       <c r="G4" s="100"/>
       <c r="H4" s="100"/>
       <c r="I4" s="105"/>
-      <c r="J4" s="124">
+      <c r="J4" s="134">
         <v>0</v>
       </c>
       <c r="K4" s="100"/>
@@ -3396,7 +3718,7 @@
       <c r="G5" s="100"/>
       <c r="H5" s="100"/>
       <c r="I5" s="105"/>
-      <c r="J5" s="124">
+      <c r="J5" s="134">
         <v>0</v>
       </c>
       <c r="K5" s="100"/>
@@ -3439,7 +3761,7 @@
       <c r="G6" s="100"/>
       <c r="H6" s="100"/>
       <c r="I6" s="105"/>
-      <c r="J6" s="124">
+      <c r="J6" s="134">
         <v>0</v>
       </c>
       <c r="K6" s="100"/>
@@ -3488,7 +3810,7 @@
       <c r="I7" s="105">
         <v>240</v>
       </c>
-      <c r="J7" s="124">
+      <c r="J7" s="134">
         <v>0</v>
       </c>
       <c r="K7" s="100" t="s">
@@ -3537,7 +3859,7 @@
       <c r="I8" s="105">
         <v>330</v>
       </c>
-      <c r="J8" s="124">
+      <c r="J8" s="134">
         <v>0</v>
       </c>
       <c r="K8" s="100" t="s">
@@ -3588,7 +3910,7 @@
       <c r="I9" s="105">
         <v>420</v>
       </c>
-      <c r="J9" s="124">
+      <c r="J9" s="134">
         <v>0</v>
       </c>
       <c r="K9" s="100" t="s">
@@ -3639,7 +3961,7 @@
       </c>
       <c r="H10" s="100"/>
       <c r="I10" s="105"/>
-      <c r="J10" s="124">
+      <c r="J10" s="134">
         <v>0</v>
       </c>
       <c r="K10" s="100" t="s">
@@ -3690,7 +4012,7 @@
       </c>
       <c r="H11" s="100"/>
       <c r="I11" s="105"/>
-      <c r="J11" s="124">
+      <c r="J11" s="134">
         <v>0</v>
       </c>
       <c r="K11" s="100" t="s">
@@ -3741,7 +4063,7 @@
       </c>
       <c r="H12" s="100"/>
       <c r="I12" s="105"/>
-      <c r="J12" s="124">
+      <c r="J12" s="134">
         <v>0</v>
       </c>
       <c r="K12" s="100"/>
@@ -3790,7 +4112,7 @@
       </c>
       <c r="H13" s="100"/>
       <c r="I13" s="105"/>
-      <c r="J13" s="124">
+      <c r="J13" s="134">
         <v>0</v>
       </c>
       <c r="K13" s="100"/>
@@ -3839,7 +4161,7 @@
       </c>
       <c r="H14" s="100"/>
       <c r="I14" s="105"/>
-      <c r="J14" s="124">
+      <c r="J14" s="134">
         <v>0</v>
       </c>
       <c r="K14" s="100" t="s">
@@ -3890,7 +4212,7 @@
       </c>
       <c r="H15" s="100"/>
       <c r="I15" s="105"/>
-      <c r="J15" s="124">
+      <c r="J15" s="134">
         <v>0</v>
       </c>
       <c r="K15" s="100" t="s">
@@ -3941,7 +4263,7 @@
       </c>
       <c r="H16" s="100"/>
       <c r="I16" s="105"/>
-      <c r="J16" s="124">
+      <c r="J16" s="134">
         <v>0</v>
       </c>
       <c r="K16" s="100" t="s">
@@ -3992,7 +4314,7 @@
       </c>
       <c r="H17" s="100"/>
       <c r="I17" s="105"/>
-      <c r="J17" s="124">
+      <c r="J17" s="134">
         <v>0</v>
       </c>
       <c r="K17" s="100"/>
@@ -4041,7 +4363,7 @@
       </c>
       <c r="H18" s="100"/>
       <c r="I18" s="105"/>
-      <c r="J18" s="124">
+      <c r="J18" s="134">
         <v>0</v>
       </c>
       <c r="K18" s="100" t="s">
@@ -4092,7 +4414,7 @@
       </c>
       <c r="H19" s="100"/>
       <c r="I19" s="105"/>
-      <c r="J19" s="124">
+      <c r="J19" s="134">
         <v>0</v>
       </c>
       <c r="K19" s="100" t="s">
@@ -4143,7 +4465,7 @@
       </c>
       <c r="H20" s="100"/>
       <c r="I20" s="105"/>
-      <c r="J20" s="124">
+      <c r="J20" s="134">
         <v>0</v>
       </c>
       <c r="K20" s="100" t="s">
@@ -4195,7 +4517,7 @@
       <c r="G21" s="100"/>
       <c r="H21" s="100"/>
       <c r="I21" s="105"/>
-      <c r="J21" s="124">
+      <c r="J21" s="134">
         <v>0</v>
       </c>
       <c r="K21" s="100"/>
@@ -4245,7 +4567,7 @@
       <c r="G22" s="100"/>
       <c r="H22" s="100"/>
       <c r="I22" s="105"/>
-      <c r="J22" s="124">
+      <c r="J22" s="134">
         <v>0</v>
       </c>
       <c r="K22" s="100"/>
@@ -4295,7 +4617,7 @@
       <c r="G23" s="100"/>
       <c r="H23" s="100"/>
       <c r="I23" s="105"/>
-      <c r="J23" s="124">
+      <c r="J23" s="134">
         <v>0</v>
       </c>
       <c r="K23" s="100"/>
@@ -4345,11 +4667,11 @@
         <v>183</v>
       </c>
       <c r="G24" s="103">
-        <v>-210</v>
+        <v>210</v>
       </c>
       <c r="H24" s="100"/>
       <c r="I24" s="105"/>
-      <c r="J24" s="124">
+      <c r="J24" s="134">
         <v>0</v>
       </c>
       <c r="K24" s="100" t="s">
@@ -4401,11 +4723,11 @@
         <v>183</v>
       </c>
       <c r="G25" s="103">
-        <v>-240</v>
+        <v>240</v>
       </c>
       <c r="H25" s="100"/>
       <c r="I25" s="105"/>
-      <c r="J25" s="124">
+      <c r="J25" s="134">
         <v>0</v>
       </c>
       <c r="K25" s="100" t="s">
@@ -4457,11 +4779,11 @@
         <v>183</v>
       </c>
       <c r="G26" s="103">
-        <v>-300</v>
+        <v>300</v>
       </c>
       <c r="H26" s="100"/>
       <c r="I26" s="105"/>
-      <c r="J26" s="124">
+      <c r="J26" s="134">
         <v>0</v>
       </c>
       <c r="K26" s="100" t="s">
@@ -4517,7 +4839,7 @@
       <c r="I27" s="105">
         <v>210</v>
       </c>
-      <c r="J27" s="124">
+      <c r="J27" s="134">
         <v>15</v>
       </c>
       <c r="K27" s="100"/>
@@ -4569,7 +4891,7 @@
       <c r="I28" s="105">
         <v>240</v>
       </c>
-      <c r="J28" s="124">
+      <c r="J28" s="134">
         <v>15</v>
       </c>
       <c r="K28" s="100"/>
@@ -4623,7 +4945,7 @@
       <c r="I29" s="105">
         <v>270</v>
       </c>
-      <c r="J29" s="124">
+      <c r="J29" s="134">
         <v>15</v>
       </c>
       <c r="K29" s="100"/>
@@ -4689,7 +5011,7 @@
       <c r="I30" s="105">
         <v>360</v>
       </c>
-      <c r="J30" s="124">
+      <c r="J30" s="134">
         <v>20</v>
       </c>
       <c r="K30" s="100"/>
@@ -4743,7 +5065,7 @@
       <c r="I31" s="105">
         <v>450</v>
       </c>
-      <c r="J31" s="124">
+      <c r="J31" s="134">
         <v>20</v>
       </c>
       <c r="K31" s="100"/>
@@ -4797,7 +5119,7 @@
       </c>
       <c r="H32" s="100"/>
       <c r="I32" s="105"/>
-      <c r="J32" s="124">
+      <c r="J32" s="134">
         <v>0</v>
       </c>
       <c r="K32" s="100" t="s">
@@ -4851,7 +5173,7 @@
       </c>
       <c r="H33" s="100"/>
       <c r="I33" s="105"/>
-      <c r="J33" s="124">
+      <c r="J33" s="134">
         <v>0</v>
       </c>
       <c r="K33" s="100" t="s">
@@ -4907,7 +5229,7 @@
       <c r="I34" s="105">
         <v>240</v>
       </c>
-      <c r="J34" s="124">
+      <c r="J34" s="134">
         <v>0</v>
       </c>
       <c r="K34" s="100"/>
@@ -4959,7 +5281,7 @@
       <c r="I35" s="105">
         <v>300</v>
       </c>
-      <c r="J35" s="124">
+      <c r="J35" s="134">
         <v>0</v>
       </c>
       <c r="K35" s="100"/>
@@ -5013,7 +5335,7 @@
       <c r="I36" s="105">
         <v>360</v>
       </c>
-      <c r="J36" s="124">
+      <c r="J36" s="134">
         <v>0</v>
       </c>
       <c r="K36" s="100"/>
@@ -5067,7 +5389,7 @@
       <c r="I37" s="105">
         <v>420</v>
       </c>
-      <c r="J37" s="124">
+      <c r="J37" s="134">
         <v>0</v>
       </c>
       <c r="K37" s="100" t="s">
@@ -5123,7 +5445,7 @@
       <c r="I38" s="105">
         <v>480</v>
       </c>
-      <c r="J38" s="124">
+      <c r="J38" s="134">
         <v>0</v>
       </c>
       <c r="K38" s="100" t="s">
@@ -5179,7 +5501,7 @@
       <c r="I39" s="105">
         <v>540</v>
       </c>
-      <c r="J39" s="124">
+      <c r="J39" s="134">
         <v>0</v>
       </c>
       <c r="K39" s="100" t="s">
@@ -5235,7 +5557,7 @@
       </c>
       <c r="H40" s="100"/>
       <c r="I40" s="105"/>
-      <c r="J40" s="124">
+      <c r="J40" s="134">
         <v>10</v>
       </c>
       <c r="K40" s="100"/>
@@ -5289,7 +5611,7 @@
       </c>
       <c r="H41" s="100"/>
       <c r="I41" s="105"/>
-      <c r="J41" s="124">
+      <c r="J41" s="134">
         <v>10</v>
       </c>
       <c r="K41" s="100"/>
@@ -5343,8 +5665,8 @@
       </c>
       <c r="H42" s="100"/>
       <c r="I42" s="105"/>
-      <c r="J42" s="124">
-        <v>15</v>
+      <c r="J42" s="134">
+        <v>25</v>
       </c>
       <c r="K42" s="100" t="s">
         <v>445</v>
@@ -5399,7 +5721,7 @@
       </c>
       <c r="H43" s="100"/>
       <c r="I43" s="105"/>
-      <c r="J43" s="124">
+      <c r="J43" s="134">
         <v>15</v>
       </c>
       <c r="K43" s="100" t="s">
@@ -5455,7 +5777,7 @@
       </c>
       <c r="H44" s="100"/>
       <c r="I44" s="105"/>
-      <c r="J44" s="124">
+      <c r="J44" s="134">
         <v>15</v>
       </c>
       <c r="K44" s="100" t="s">
@@ -5507,8 +5829,8 @@
       <c r="G45" s="100"/>
       <c r="H45" s="100"/>
       <c r="I45" s="105"/>
-      <c r="J45" s="124">
-        <v>15</v>
+      <c r="J45" s="134">
+        <v>-15</v>
       </c>
       <c r="K45" s="100"/>
       <c r="L45" s="118" t="s">
@@ -5555,8 +5877,8 @@
       <c r="G46" s="100"/>
       <c r="H46" s="100"/>
       <c r="I46" s="105"/>
-      <c r="J46" s="124">
-        <v>15</v>
+      <c r="J46" s="134">
+        <v>-15</v>
       </c>
       <c r="K46" s="100" t="s">
         <v>441</v>
@@ -5605,7 +5927,7 @@
       <c r="G47" s="100"/>
       <c r="H47" s="100"/>
       <c r="I47" s="105"/>
-      <c r="J47" s="124">
+      <c r="J47" s="134">
         <v>0</v>
       </c>
       <c r="K47" s="100"/>
@@ -5651,7 +5973,7 @@
       <c r="G48" s="100"/>
       <c r="H48" s="100"/>
       <c r="I48" s="105"/>
-      <c r="J48" s="124">
+      <c r="J48" s="134">
         <v>0</v>
       </c>
       <c r="K48" s="100"/>
@@ -5695,7 +6017,7 @@
       <c r="G49" s="100"/>
       <c r="H49" s="100"/>
       <c r="I49" s="105"/>
-      <c r="J49" s="124">
+      <c r="J49" s="134">
         <v>0</v>
       </c>
       <c r="K49" s="100"/>
@@ -5741,7 +6063,7 @@
       <c r="G50" s="100"/>
       <c r="H50" s="100"/>
       <c r="I50" s="105"/>
-      <c r="J50" s="124">
+      <c r="J50" s="134">
         <v>0</v>
       </c>
       <c r="K50" s="100"/>
@@ -5789,7 +6111,7 @@
       <c r="G51" s="100"/>
       <c r="H51" s="100"/>
       <c r="I51" s="105"/>
-      <c r="J51" s="124">
+      <c r="J51" s="134">
         <v>0</v>
       </c>
       <c r="K51" s="100"/>
@@ -5837,11 +6159,11 @@
         <v>69</v>
       </c>
       <c r="G52" s="103">
-        <v>-180</v>
+        <v>180</v>
       </c>
       <c r="H52" s="100"/>
       <c r="I52" s="105"/>
-      <c r="J52" s="124">
+      <c r="J52" s="134">
         <v>0</v>
       </c>
       <c r="K52" s="100" t="s">
@@ -5891,11 +6213,11 @@
         <v>69</v>
       </c>
       <c r="G53" s="103">
-        <v>-240</v>
+        <v>240</v>
       </c>
       <c r="H53" s="100"/>
       <c r="I53" s="105"/>
-      <c r="J53" s="124">
+      <c r="J53" s="134">
         <v>0</v>
       </c>
       <c r="K53" s="100" t="s">
@@ -5957,11 +6279,11 @@
         <v>69</v>
       </c>
       <c r="G54" s="103">
-        <v>-300</v>
+        <v>300</v>
       </c>
       <c r="H54" s="100"/>
       <c r="I54" s="105"/>
-      <c r="J54" s="124">
+      <c r="J54" s="134">
         <v>0</v>
       </c>
       <c r="K54" s="100" t="s">
@@ -6017,7 +6339,7 @@
       </c>
       <c r="H55" s="100"/>
       <c r="I55" s="105"/>
-      <c r="J55" s="124">
+      <c r="J55" s="134">
         <v>0</v>
       </c>
       <c r="K55" s="100" t="s">
@@ -6073,7 +6395,7 @@
       </c>
       <c r="H56" s="100"/>
       <c r="I56" s="105"/>
-      <c r="J56" s="124">
+      <c r="J56" s="134">
         <v>0</v>
       </c>
       <c r="K56" s="100" t="s">
@@ -6129,8 +6451,8 @@
       </c>
       <c r="H57" s="100"/>
       <c r="I57" s="105"/>
-      <c r="J57" s="124">
-        <v>30</v>
+      <c r="J57" s="134">
+        <v>-30</v>
       </c>
       <c r="K57" s="100"/>
       <c r="L57" s="118" t="s">
@@ -6183,8 +6505,8 @@
       </c>
       <c r="H58" s="100"/>
       <c r="I58" s="105"/>
-      <c r="J58" s="124">
-        <v>30</v>
+      <c r="J58" s="134">
+        <v>-30</v>
       </c>
       <c r="K58" s="100"/>
       <c r="L58" s="118" t="s">
@@ -6237,8 +6559,8 @@
       </c>
       <c r="H59" s="100"/>
       <c r="I59" s="105"/>
-      <c r="J59" s="124">
-        <v>30</v>
+      <c r="J59" s="134">
+        <v>-30</v>
       </c>
       <c r="K59" s="100"/>
       <c r="L59" s="118" t="s">
@@ -6291,7 +6613,7 @@
       </c>
       <c r="H60" s="100"/>
       <c r="I60" s="105"/>
-      <c r="J60" s="124">
+      <c r="J60" s="134">
         <v>0</v>
       </c>
       <c r="K60" s="100"/>
@@ -6345,7 +6667,7 @@
       </c>
       <c r="H61" s="100"/>
       <c r="I61" s="105"/>
-      <c r="J61" s="124">
+      <c r="J61" s="134">
         <v>0</v>
       </c>
       <c r="K61" s="100"/>
@@ -6399,7 +6721,7 @@
       </c>
       <c r="H62" s="100"/>
       <c r="I62" s="105"/>
-      <c r="J62" s="124">
+      <c r="J62" s="134">
         <v>0</v>
       </c>
       <c r="K62" s="100"/>
@@ -6453,7 +6775,7 @@
       </c>
       <c r="H63" s="100"/>
       <c r="I63" s="105"/>
-      <c r="J63" s="124">
+      <c r="J63" s="134">
         <v>0</v>
       </c>
       <c r="K63" s="100" t="s">
@@ -6509,7 +6831,7 @@
       </c>
       <c r="H64" s="100"/>
       <c r="I64" s="105"/>
-      <c r="J64" s="124">
+      <c r="J64" s="134">
         <v>0</v>
       </c>
       <c r="K64" s="100" t="s">
@@ -6565,7 +6887,7 @@
       </c>
       <c r="H65" s="100"/>
       <c r="I65" s="105"/>
-      <c r="J65" s="124">
+      <c r="J65" s="134">
         <v>0</v>
       </c>
       <c r="K65" s="100" t="s">
@@ -6617,8 +6939,8 @@
       <c r="G66" s="100"/>
       <c r="H66" s="100"/>
       <c r="I66" s="105"/>
-      <c r="J66" s="124">
-        <v>20</v>
+      <c r="J66" s="134">
+        <v>-20</v>
       </c>
       <c r="K66" s="100"/>
       <c r="L66" s="118" t="s">
@@ -6665,8 +6987,8 @@
       <c r="G67" s="100"/>
       <c r="H67" s="100"/>
       <c r="I67" s="105"/>
-      <c r="J67" s="124">
-        <v>20</v>
+      <c r="J67" s="134">
+        <v>-20</v>
       </c>
       <c r="K67" s="100"/>
       <c r="L67" s="118" t="s">
@@ -6715,8 +7037,8 @@
       <c r="G68" s="100"/>
       <c r="H68" s="100"/>
       <c r="I68" s="105"/>
-      <c r="J68" s="124">
-        <v>20</v>
+      <c r="J68" s="134">
+        <v>-20</v>
       </c>
       <c r="K68" s="100"/>
       <c r="L68" s="118" t="s">
@@ -6769,8 +7091,8 @@
       <c r="I69" s="105">
         <v>270</v>
       </c>
-      <c r="J69" s="124">
-        <v>20</v>
+      <c r="J69" s="134">
+        <v>-20</v>
       </c>
       <c r="K69" s="100" t="s">
         <v>457</v>
@@ -6825,8 +7147,8 @@
       <c r="I70" s="105">
         <v>330</v>
       </c>
-      <c r="J70" s="124">
-        <v>20</v>
+      <c r="J70" s="134">
+        <v>-20</v>
       </c>
       <c r="K70" s="100" t="s">
         <v>441</v>
@@ -6881,8 +7203,8 @@
       <c r="I71" s="105">
         <v>390</v>
       </c>
-      <c r="J71" s="124">
-        <v>20</v>
+      <c r="J71" s="134">
+        <v>-20</v>
       </c>
       <c r="K71" s="100" t="s">
         <v>458</v>
@@ -6937,7 +7259,7 @@
       <c r="I72" s="105">
         <v>150</v>
       </c>
-      <c r="J72" s="124">
+      <c r="J72" s="134">
         <v>0</v>
       </c>
       <c r="K72" s="100"/>
@@ -6989,7 +7311,7 @@
       <c r="I73" s="105">
         <v>180</v>
       </c>
-      <c r="J73" s="124">
+      <c r="J73" s="134">
         <v>0</v>
       </c>
       <c r="K73" s="100"/>
@@ -7043,7 +7365,7 @@
       <c r="I74" s="105">
         <v>210</v>
       </c>
-      <c r="J74" s="124">
+      <c r="J74" s="134">
         <v>0</v>
       </c>
       <c r="K74" s="100"/>
@@ -7097,7 +7419,7 @@
       <c r="I75" s="105">
         <v>240</v>
       </c>
-      <c r="J75" s="124">
+      <c r="J75" s="134">
         <v>0</v>
       </c>
       <c r="K75" s="100"/>
@@ -7151,7 +7473,7 @@
       <c r="I76" s="105">
         <v>270</v>
       </c>
-      <c r="J76" s="124">
+      <c r="J76" s="134">
         <v>0</v>
       </c>
       <c r="K76" s="100"/>
@@ -7205,7 +7527,7 @@
       </c>
       <c r="H77" s="100"/>
       <c r="I77" s="105"/>
-      <c r="J77" s="124">
+      <c r="J77" s="134">
         <v>0</v>
       </c>
       <c r="K77" s="100"/>
@@ -7263,7 +7585,7 @@
       </c>
       <c r="H78" s="100"/>
       <c r="I78" s="105"/>
-      <c r="J78" s="124">
+      <c r="J78" s="134">
         <v>0</v>
       </c>
       <c r="K78" s="100"/>
@@ -7315,7 +7637,7 @@
       </c>
       <c r="H79" s="100"/>
       <c r="I79" s="105"/>
-      <c r="J79" s="124">
+      <c r="J79" s="134">
         <v>0</v>
       </c>
       <c r="K79" s="100" t="s">
@@ -7371,7 +7693,7 @@
       </c>
       <c r="H80" s="100"/>
       <c r="I80" s="105"/>
-      <c r="J80" s="124">
+      <c r="J80" s="134">
         <v>0</v>
       </c>
       <c r="K80" s="100"/>
@@ -7425,7 +7747,7 @@
       </c>
       <c r="H81" s="100"/>
       <c r="I81" s="105"/>
-      <c r="J81" s="124">
+      <c r="J81" s="134">
         <v>0</v>
       </c>
       <c r="K81" s="100"/>
@@ -7479,7 +7801,7 @@
       </c>
       <c r="H82" s="100"/>
       <c r="I82" s="105"/>
-      <c r="J82" s="124">
+      <c r="J82" s="134">
         <v>0</v>
       </c>
       <c r="K82" s="100"/>
@@ -7533,8 +7855,8 @@
       <c r="I83" s="105">
         <v>330</v>
       </c>
-      <c r="J83" s="124">
-        <v>20</v>
+      <c r="J83" s="134">
+        <v>-20</v>
       </c>
       <c r="K83" s="100" t="s">
         <v>456</v>
@@ -7589,8 +7911,8 @@
       <c r="I84" s="105">
         <v>420</v>
       </c>
-      <c r="J84" s="124">
-        <v>20</v>
+      <c r="J84" s="134">
+        <v>-20</v>
       </c>
       <c r="K84" s="100" t="s">
         <v>459</v>
@@ -7645,7 +7967,7 @@
       </c>
       <c r="H85" s="100"/>
       <c r="I85" s="105"/>
-      <c r="J85" s="124">
+      <c r="J85" s="134">
         <v>10</v>
       </c>
       <c r="K85" s="100"/>
@@ -7703,7 +8025,7 @@
       </c>
       <c r="H86" s="100"/>
       <c r="I86" s="105"/>
-      <c r="J86" s="124">
+      <c r="J86" s="134">
         <v>10</v>
       </c>
       <c r="K86" s="100"/>
@@ -7757,7 +8079,7 @@
       </c>
       <c r="H87" s="100"/>
       <c r="I87" s="105"/>
-      <c r="J87" s="124">
+      <c r="J87" s="134">
         <v>0</v>
       </c>
       <c r="K87" s="100" t="s">
@@ -7813,7 +8135,7 @@
       </c>
       <c r="H88" s="100"/>
       <c r="I88" s="105"/>
-      <c r="J88" s="124">
+      <c r="J88" s="134">
         <v>10</v>
       </c>
       <c r="K88" s="100" t="s">
@@ -7869,7 +8191,7 @@
       </c>
       <c r="H89" s="100"/>
       <c r="I89" s="105"/>
-      <c r="J89" s="124">
+      <c r="J89" s="134">
         <v>15</v>
       </c>
       <c r="K89" s="100" t="s">
@@ -7925,7 +8247,7 @@
       <c r="I90" s="105">
         <v>240</v>
       </c>
-      <c r="J90" s="124">
+      <c r="J90" s="134">
         <v>0</v>
       </c>
       <c r="K90" s="100" t="s">
@@ -7973,7 +8295,7 @@
       <c r="I91" s="105">
         <v>330</v>
       </c>
-      <c r="J91" s="124">
+      <c r="J91" s="134">
         <v>0</v>
       </c>
       <c r="K91" s="100" t="s">
@@ -8006,14 +8328,2341 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:K80"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="R39" sqref="R39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.500000"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:11">
+      <c r="A1" s="123" t="s">
+        <v>478</v>
+      </c>
+      <c r="B1" s="124">
+        <v>1</v>
+      </c>
+      <c r="C1" s="123" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="125">
+        <v>264</v>
+      </c>
+      <c r="E1" s="126">
+        <v>0</v>
+      </c>
+      <c r="F1" s="127"/>
+      <c r="G1" s="128"/>
+      <c r="H1" s="128"/>
+      <c r="I1" s="128"/>
+      <c r="J1" s="129">
+        <v>0</v>
+      </c>
+      <c r="K1" s="126"/>
+    </row>
+    <row r="2" spans="1:11">
+      <c r="A2" s="123" t="s">
+        <v>479</v>
+      </c>
+      <c r="B2" s="124">
+        <v>1</v>
+      </c>
+      <c r="C2" s="123" t="s">
+        <v>421</v>
+      </c>
+      <c r="D2" s="125">
+        <v>297</v>
+      </c>
+      <c r="E2" s="126">
+        <v>0</v>
+      </c>
+      <c r="F2" s="127"/>
+      <c r="G2" s="128"/>
+      <c r="H2" s="128"/>
+      <c r="I2" s="128"/>
+      <c r="J2" s="129">
+        <v>0</v>
+      </c>
+      <c r="K2" s="126"/>
+    </row>
+    <row r="3" spans="1:11">
+      <c r="A3" s="123" t="s">
+        <v>480</v>
+      </c>
+      <c r="B3" s="124">
+        <v>2</v>
+      </c>
+      <c r="C3" s="123" t="s">
+        <v>421</v>
+      </c>
+      <c r="D3" s="125">
+        <v>330</v>
+      </c>
+      <c r="E3" s="126">
+        <v>0</v>
+      </c>
+      <c r="F3" s="127"/>
+      <c r="G3" s="128"/>
+      <c r="H3" s="128"/>
+      <c r="I3" s="128"/>
+      <c r="J3" s="129">
+        <v>0</v>
+      </c>
+      <c r="K3" s="126"/>
+    </row>
+    <row r="4" spans="1:11">
+      <c r="A4" s="123" t="s">
+        <v>481</v>
+      </c>
+      <c r="B4" s="124">
+        <v>3</v>
+      </c>
+      <c r="C4" s="123" t="s">
+        <v>421</v>
+      </c>
+      <c r="D4" s="125">
+        <v>363</v>
+      </c>
+      <c r="E4" s="126">
+        <v>0</v>
+      </c>
+      <c r="F4" s="127"/>
+      <c r="G4" s="128"/>
+      <c r="H4" s="128"/>
+      <c r="I4" s="128"/>
+      <c r="J4" s="129">
+        <v>0</v>
+      </c>
+      <c r="K4" s="126"/>
+    </row>
+    <row r="5" spans="1:11">
+      <c r="A5" s="123" t="s">
+        <v>482</v>
+      </c>
+      <c r="B5" s="124">
+        <v>4</v>
+      </c>
+      <c r="C5" s="123" t="s">
+        <v>421</v>
+      </c>
+      <c r="D5" s="125">
+        <v>429</v>
+      </c>
+      <c r="E5" s="126">
+        <v>0</v>
+      </c>
+      <c r="F5" s="127"/>
+      <c r="G5" s="128"/>
+      <c r="H5" s="128"/>
+      <c r="I5" s="128"/>
+      <c r="J5" s="129">
+        <v>0</v>
+      </c>
+      <c r="K5" s="126"/>
+    </row>
+    <row r="6" spans="1:11">
+      <c r="A6" s="123" t="s">
+        <v>483</v>
+      </c>
+      <c r="B6" s="124">
+        <v>5</v>
+      </c>
+      <c r="C6" s="123" t="s">
+        <v>421</v>
+      </c>
+      <c r="D6" s="125">
+        <v>462</v>
+      </c>
+      <c r="E6" s="126">
+        <v>0</v>
+      </c>
+      <c r="F6" s="127" t="s">
+        <v>183</v>
+      </c>
+      <c r="G6" s="130">
+        <v>120</v>
+      </c>
+      <c r="H6" s="128"/>
+      <c r="I6" s="128"/>
+      <c r="J6" s="129">
+        <v>0</v>
+      </c>
+      <c r="K6" s="126" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11">
+      <c r="A7" s="123" t="s">
+        <v>484</v>
+      </c>
+      <c r="B7" s="124">
+        <v>6</v>
+      </c>
+      <c r="C7" s="123" t="s">
+        <v>421</v>
+      </c>
+      <c r="D7" s="125">
+        <v>528</v>
+      </c>
+      <c r="E7" s="126">
+        <v>0</v>
+      </c>
+      <c r="F7" s="127" t="s">
+        <v>183</v>
+      </c>
+      <c r="G7" s="130">
+        <v>150</v>
+      </c>
+      <c r="H7" s="128"/>
+      <c r="I7" s="128"/>
+      <c r="J7" s="129">
+        <v>0</v>
+      </c>
+      <c r="K7" s="126" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
+      <c r="A8" s="123" t="s">
+        <v>485</v>
+      </c>
+      <c r="B8" s="124">
+        <v>6</v>
+      </c>
+      <c r="C8" s="123" t="s">
+        <v>421</v>
+      </c>
+      <c r="D8" s="125">
+        <v>594</v>
+      </c>
+      <c r="E8" s="126">
+        <v>0</v>
+      </c>
+      <c r="F8" s="127" t="s">
+        <v>183</v>
+      </c>
+      <c r="G8" s="130">
+        <v>180</v>
+      </c>
+      <c r="H8" s="128"/>
+      <c r="I8" s="128"/>
+      <c r="J8" s="129">
+        <v>0</v>
+      </c>
+      <c r="K8" s="126" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11">
+      <c r="A9" s="123" t="s">
+        <v>486</v>
+      </c>
+      <c r="B9" s="124">
+        <v>7</v>
+      </c>
+      <c r="C9" s="123" t="s">
+        <v>421</v>
+      </c>
+      <c r="D9" s="125">
+        <v>627</v>
+      </c>
+      <c r="E9" s="126">
+        <v>0</v>
+      </c>
+      <c r="F9" s="127" t="s">
+        <v>2</v>
+      </c>
+      <c r="G9" s="128" t="s">
+        <v>487</v>
+      </c>
+      <c r="H9" s="128"/>
+      <c r="I9" s="128"/>
+      <c r="J9" s="129">
+        <v>0</v>
+      </c>
+      <c r="K9" s="126" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11">
+      <c r="A10" s="123" t="s">
+        <v>488</v>
+      </c>
+      <c r="B10" s="124">
+        <v>8</v>
+      </c>
+      <c r="C10" s="123" t="s">
+        <v>421</v>
+      </c>
+      <c r="D10" s="125">
+        <v>693</v>
+      </c>
+      <c r="E10" s="126">
+        <v>0</v>
+      </c>
+      <c r="F10" s="127" t="s">
+        <v>2</v>
+      </c>
+      <c r="G10" s="128" t="s">
+        <v>489</v>
+      </c>
+      <c r="H10" s="128"/>
+      <c r="I10" s="128"/>
+      <c r="J10" s="129">
+        <v>0</v>
+      </c>
+      <c r="K10" s="126" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11">
+      <c r="A11" s="123" t="s">
+        <v>490</v>
+      </c>
+      <c r="B11" s="124">
+        <v>3</v>
+      </c>
+      <c r="C11" s="123" t="s">
+        <v>421</v>
+      </c>
+      <c r="D11" s="125">
+        <v>429</v>
+      </c>
+      <c r="E11" s="126">
+        <v>0</v>
+      </c>
+      <c r="F11" s="127"/>
+      <c r="G11" s="128"/>
+      <c r="H11" s="128"/>
+      <c r="I11" s="128"/>
+      <c r="J11" s="129">
+        <v>0</v>
+      </c>
+      <c r="K11" s="126"/>
+    </row>
+    <row r="12" spans="1:11">
+      <c r="A12" s="123" t="s">
+        <v>491</v>
+      </c>
+      <c r="B12" s="124">
+        <v>4</v>
+      </c>
+      <c r="C12" s="123" t="s">
+        <v>421</v>
+      </c>
+      <c r="D12" s="125">
+        <v>462</v>
+      </c>
+      <c r="E12" s="126">
+        <v>0</v>
+      </c>
+      <c r="F12" s="127"/>
+      <c r="G12" s="128"/>
+      <c r="H12" s="128"/>
+      <c r="I12" s="128"/>
+      <c r="J12" s="129">
+        <v>0</v>
+      </c>
+      <c r="K12" s="126"/>
+    </row>
+    <row r="13" spans="1:11">
+      <c r="A13" s="123" t="s">
+        <v>492</v>
+      </c>
+      <c r="B13" s="124">
+        <v>5</v>
+      </c>
+      <c r="C13" s="123" t="s">
+        <v>421</v>
+      </c>
+      <c r="D13" s="125">
+        <v>528</v>
+      </c>
+      <c r="E13" s="126">
+        <v>0</v>
+      </c>
+      <c r="F13" s="127" t="s">
+        <v>27</v>
+      </c>
+      <c r="G13" s="130">
+        <v>240</v>
+      </c>
+      <c r="H13" s="128"/>
+      <c r="I13" s="128"/>
+      <c r="J13" s="129">
+        <v>0</v>
+      </c>
+      <c r="K13" s="126" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11">
+      <c r="A14" s="123" t="s">
+        <v>493</v>
+      </c>
+      <c r="B14" s="124">
+        <v>6</v>
+      </c>
+      <c r="C14" s="123" t="s">
+        <v>421</v>
+      </c>
+      <c r="D14" s="125">
+        <v>561</v>
+      </c>
+      <c r="E14" s="126">
+        <v>0</v>
+      </c>
+      <c r="F14" s="127" t="s">
+        <v>27</v>
+      </c>
+      <c r="G14" s="130">
+        <v>300</v>
+      </c>
+      <c r="H14" s="128"/>
+      <c r="I14" s="128"/>
+      <c r="J14" s="129">
+        <v>0</v>
+      </c>
+      <c r="K14" s="126" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11">
+      <c r="A15" s="123" t="s">
+        <v>494</v>
+      </c>
+      <c r="B15" s="124">
+        <v>6</v>
+      </c>
+      <c r="C15" s="123" t="s">
+        <v>421</v>
+      </c>
+      <c r="D15" s="125">
+        <v>594</v>
+      </c>
+      <c r="E15" s="126">
+        <v>0</v>
+      </c>
+      <c r="F15" s="127" t="s">
+        <v>27</v>
+      </c>
+      <c r="G15" s="130">
+        <v>360</v>
+      </c>
+      <c r="H15" s="128"/>
+      <c r="I15" s="128"/>
+      <c r="J15" s="129">
+        <v>0</v>
+      </c>
+      <c r="K15" s="126" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11">
+      <c r="A16" s="123" t="s">
+        <v>495</v>
+      </c>
+      <c r="B16" s="124">
+        <v>2</v>
+      </c>
+      <c r="C16" s="123" t="s">
+        <v>421</v>
+      </c>
+      <c r="D16" s="125">
+        <v>330</v>
+      </c>
+      <c r="E16" s="126">
+        <v>0</v>
+      </c>
+      <c r="F16" s="127"/>
+      <c r="G16" s="128"/>
+      <c r="H16" s="128"/>
+      <c r="I16" s="128"/>
+      <c r="J16" s="129">
+        <v>0</v>
+      </c>
+      <c r="K16" s="126"/>
+    </row>
+    <row r="17" spans="1:11">
+      <c r="A17" s="123" t="s">
+        <v>496</v>
+      </c>
+      <c r="B17" s="124">
+        <v>3</v>
+      </c>
+      <c r="C17" s="123" t="s">
+        <v>421</v>
+      </c>
+      <c r="D17" s="125">
+        <v>363</v>
+      </c>
+      <c r="E17" s="126">
+        <v>0</v>
+      </c>
+      <c r="F17" s="127"/>
+      <c r="G17" s="128"/>
+      <c r="H17" s="128"/>
+      <c r="I17" s="128"/>
+      <c r="J17" s="129">
+        <v>15</v>
+      </c>
+      <c r="K17" s="126"/>
+    </row>
+    <row r="18" spans="1:11">
+      <c r="A18" s="123" t="s">
+        <v>497</v>
+      </c>
+      <c r="B18" s="124">
+        <v>4</v>
+      </c>
+      <c r="C18" s="123" t="s">
+        <v>421</v>
+      </c>
+      <c r="D18" s="125">
+        <v>429</v>
+      </c>
+      <c r="E18" s="126">
+        <v>0</v>
+      </c>
+      <c r="F18" s="127"/>
+      <c r="G18" s="128"/>
+      <c r="H18" s="128"/>
+      <c r="I18" s="128"/>
+      <c r="J18" s="129">
+        <v>15</v>
+      </c>
+      <c r="K18" s="126"/>
+    </row>
+    <row r="19" spans="1:11">
+      <c r="A19" s="124" t="s">
+        <v>498</v>
+      </c>
+      <c r="B19" s="124">
+        <v>5</v>
+      </c>
+      <c r="C19" s="123" t="s">
+        <v>421</v>
+      </c>
+      <c r="D19" s="125">
+        <v>495</v>
+      </c>
+      <c r="E19" s="126">
+        <v>0</v>
+      </c>
+      <c r="F19" s="127"/>
+      <c r="G19" s="128"/>
+      <c r="H19" s="128" t="s">
+        <v>436</v>
+      </c>
+      <c r="I19" s="128">
+        <v>210</v>
+      </c>
+      <c r="J19" s="129">
+        <v>20</v>
+      </c>
+      <c r="K19" s="126"/>
+    </row>
+    <row r="20" spans="1:11">
+      <c r="A20" s="124" t="s">
+        <v>499</v>
+      </c>
+      <c r="B20" s="124">
+        <v>6</v>
+      </c>
+      <c r="C20" s="123" t="s">
+        <v>421</v>
+      </c>
+      <c r="D20" s="125">
+        <v>528</v>
+      </c>
+      <c r="E20" s="126">
+        <v>0</v>
+      </c>
+      <c r="F20" s="127"/>
+      <c r="G20" s="128"/>
+      <c r="H20" s="128" t="s">
+        <v>436</v>
+      </c>
+      <c r="I20" s="128">
+        <v>240</v>
+      </c>
+      <c r="J20" s="129">
+        <v>20</v>
+      </c>
+      <c r="K20" s="126"/>
+    </row>
+    <row r="21" spans="1:11">
+      <c r="A21" s="124" t="s">
+        <v>500</v>
+      </c>
+      <c r="B21" s="124">
+        <v>6</v>
+      </c>
+      <c r="C21" s="123" t="s">
+        <v>421</v>
+      </c>
+      <c r="D21" s="125">
+        <v>561</v>
+      </c>
+      <c r="E21" s="126">
+        <v>0</v>
+      </c>
+      <c r="F21" s="127"/>
+      <c r="G21" s="128"/>
+      <c r="H21" s="128" t="s">
+        <v>436</v>
+      </c>
+      <c r="I21" s="128">
+        <v>270</v>
+      </c>
+      <c r="J21" s="129">
+        <v>20</v>
+      </c>
+      <c r="K21" s="126"/>
+    </row>
+    <row r="22" spans="1:11">
+      <c r="A22" s="123" t="s">
+        <v>501</v>
+      </c>
+      <c r="B22" s="124">
+        <v>6</v>
+      </c>
+      <c r="C22" s="123" t="s">
+        <v>421</v>
+      </c>
+      <c r="D22" s="125">
+        <v>594</v>
+      </c>
+      <c r="E22" s="126">
+        <v>25</v>
+      </c>
+      <c r="F22" s="127" t="s">
+        <v>228</v>
+      </c>
+      <c r="G22" s="128">
+        <v>90</v>
+      </c>
+      <c r="H22" s="128"/>
+      <c r="I22" s="128"/>
+      <c r="J22" s="129">
+        <v>-10</v>
+      </c>
+      <c r="K22" s="126" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11">
+      <c r="A23" s="123" t="s">
+        <v>502</v>
+      </c>
+      <c r="B23" s="124">
+        <v>7</v>
+      </c>
+      <c r="C23" s="123" t="s">
+        <v>421</v>
+      </c>
+      <c r="D23" s="125">
+        <v>660</v>
+      </c>
+      <c r="E23" s="126">
+        <v>30</v>
+      </c>
+      <c r="F23" s="127" t="s">
+        <v>228</v>
+      </c>
+      <c r="G23" s="128">
+        <v>120</v>
+      </c>
+      <c r="H23" s="128"/>
+      <c r="I23" s="128"/>
+      <c r="J23" s="129">
+        <v>-10</v>
+      </c>
+      <c r="K23" s="126" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11">
+      <c r="A24" s="123" t="s">
+        <v>504</v>
+      </c>
+      <c r="B24" s="124">
+        <v>3</v>
+      </c>
+      <c r="C24" s="123" t="s">
+        <v>421</v>
+      </c>
+      <c r="D24" s="125">
+        <v>363</v>
+      </c>
+      <c r="E24" s="126">
+        <v>0</v>
+      </c>
+      <c r="F24" s="127"/>
+      <c r="G24" s="128"/>
+      <c r="H24" s="128" t="s">
+        <v>434</v>
+      </c>
+      <c r="I24" s="128">
+        <v>240</v>
+      </c>
+      <c r="J24" s="129">
+        <v>10</v>
+      </c>
+      <c r="K24" s="126"/>
+    </row>
+    <row r="25" spans="1:11">
+      <c r="A25" s="123" t="s">
+        <v>505</v>
+      </c>
+      <c r="B25" s="124">
+        <v>5</v>
+      </c>
+      <c r="C25" s="123" t="s">
+        <v>421</v>
+      </c>
+      <c r="D25" s="125">
+        <v>495</v>
+      </c>
+      <c r="E25" s="126">
+        <v>0</v>
+      </c>
+      <c r="F25" s="127"/>
+      <c r="G25" s="128"/>
+      <c r="H25" s="128" t="s">
+        <v>434</v>
+      </c>
+      <c r="I25" s="128">
+        <v>270</v>
+      </c>
+      <c r="J25" s="129">
+        <v>10</v>
+      </c>
+      <c r="K25" s="126" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11">
+      <c r="A26" s="123" t="s">
+        <v>506</v>
+      </c>
+      <c r="B26" s="124">
+        <v>7</v>
+      </c>
+      <c r="C26" s="123" t="s">
+        <v>421</v>
+      </c>
+      <c r="D26" s="125">
+        <v>627</v>
+      </c>
+      <c r="E26" s="126">
+        <v>0</v>
+      </c>
+      <c r="F26" s="127"/>
+      <c r="G26" s="128"/>
+      <c r="H26" s="128" t="s">
+        <v>434</v>
+      </c>
+      <c r="I26" s="128">
+        <v>33</v>
+      </c>
+      <c r="J26" s="129">
+        <v>10</v>
+      </c>
+      <c r="K26" s="126" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11">
+      <c r="A27" s="123" t="s">
+        <v>507</v>
+      </c>
+      <c r="B27" s="124">
+        <v>4</v>
+      </c>
+      <c r="C27" s="123" t="s">
+        <v>421</v>
+      </c>
+      <c r="D27" s="125">
+        <v>396</v>
+      </c>
+      <c r="E27" s="126">
+        <v>0</v>
+      </c>
+      <c r="F27" s="127" t="s">
+        <v>228</v>
+      </c>
+      <c r="G27" s="128">
+        <v>150</v>
+      </c>
+      <c r="H27" s="128"/>
+      <c r="I27" s="128"/>
+      <c r="J27" s="129">
+        <v>15</v>
+      </c>
+      <c r="K27" s="126"/>
+    </row>
+    <row r="28" spans="1:11">
+      <c r="A28" s="123" t="s">
+        <v>508</v>
+      </c>
+      <c r="B28" s="124">
+        <v>6</v>
+      </c>
+      <c r="C28" s="123" t="s">
+        <v>421</v>
+      </c>
+      <c r="D28" s="125">
+        <v>528</v>
+      </c>
+      <c r="E28" s="126">
+        <v>0</v>
+      </c>
+      <c r="F28" s="127" t="s">
+        <v>228</v>
+      </c>
+      <c r="G28" s="128">
+        <v>180</v>
+      </c>
+      <c r="H28" s="128"/>
+      <c r="I28" s="128"/>
+      <c r="J28" s="129">
+        <v>15</v>
+      </c>
+      <c r="K28" s="126" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11">
+      <c r="A29" s="123" t="s">
+        <v>509</v>
+      </c>
+      <c r="B29" s="124">
+        <v>7</v>
+      </c>
+      <c r="C29" s="123" t="s">
+        <v>421</v>
+      </c>
+      <c r="D29" s="125">
+        <v>561</v>
+      </c>
+      <c r="E29" s="126">
+        <v>0</v>
+      </c>
+      <c r="F29" s="127" t="s">
+        <v>228</v>
+      </c>
+      <c r="G29" s="128">
+        <v>210</v>
+      </c>
+      <c r="H29" s="128"/>
+      <c r="I29" s="128"/>
+      <c r="J29" s="129">
+        <v>15</v>
+      </c>
+      <c r="K29" s="126" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11">
+      <c r="A30" s="123" t="s">
+        <v>510</v>
+      </c>
+      <c r="B30" s="124">
+        <v>8</v>
+      </c>
+      <c r="C30" s="123" t="s">
+        <v>421</v>
+      </c>
+      <c r="D30" s="125">
+        <v>627</v>
+      </c>
+      <c r="E30" s="126">
+        <v>0</v>
+      </c>
+      <c r="F30" s="127" t="s">
+        <v>228</v>
+      </c>
+      <c r="G30" s="128">
+        <v>240</v>
+      </c>
+      <c r="H30" s="128"/>
+      <c r="I30" s="128"/>
+      <c r="J30" s="129">
+        <v>15</v>
+      </c>
+      <c r="K30" s="126" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11">
+      <c r="A31" s="123" t="s">
+        <v>511</v>
+      </c>
+      <c r="B31" s="124">
+        <v>1</v>
+      </c>
+      <c r="C31" s="123" t="s">
+        <v>1</v>
+      </c>
+      <c r="D31" s="125">
+        <v>297</v>
+      </c>
+      <c r="E31" s="126">
+        <v>0</v>
+      </c>
+      <c r="F31" s="127"/>
+      <c r="G31" s="128"/>
+      <c r="H31" s="128"/>
+      <c r="I31" s="128"/>
+      <c r="J31" s="129">
+        <v>0</v>
+      </c>
+      <c r="K31" s="126"/>
+    </row>
+    <row r="32" spans="1:11">
+      <c r="A32" s="123" t="s">
+        <v>512</v>
+      </c>
+      <c r="B32" s="124">
+        <v>1</v>
+      </c>
+      <c r="C32" s="123" t="s">
+        <v>421</v>
+      </c>
+      <c r="D32" s="125">
+        <v>330</v>
+      </c>
+      <c r="E32" s="126">
+        <v>0</v>
+      </c>
+      <c r="F32" s="127"/>
+      <c r="G32" s="128"/>
+      <c r="H32" s="128"/>
+      <c r="I32" s="128"/>
+      <c r="J32" s="129">
+        <v>0</v>
+      </c>
+      <c r="K32" s="126"/>
+    </row>
+    <row r="33" spans="1:11">
+      <c r="A33" s="123" t="s">
+        <v>513</v>
+      </c>
+      <c r="B33" s="124">
+        <v>2</v>
+      </c>
+      <c r="C33" s="123" t="s">
+        <v>421</v>
+      </c>
+      <c r="D33" s="125">
+        <v>396</v>
+      </c>
+      <c r="E33" s="126">
+        <v>0</v>
+      </c>
+      <c r="F33" s="127"/>
+      <c r="G33" s="128"/>
+      <c r="H33" s="128"/>
+      <c r="I33" s="128"/>
+      <c r="J33" s="129">
+        <v>0</v>
+      </c>
+      <c r="K33" s="126"/>
+    </row>
+    <row r="34" spans="1:11">
+      <c r="A34" s="123" t="s">
+        <v>514</v>
+      </c>
+      <c r="B34" s="124">
+        <v>3</v>
+      </c>
+      <c r="C34" s="123" t="s">
+        <v>421</v>
+      </c>
+      <c r="D34" s="125">
+        <v>429</v>
+      </c>
+      <c r="E34" s="126">
+        <v>0</v>
+      </c>
+      <c r="F34" s="127"/>
+      <c r="G34" s="128"/>
+      <c r="H34" s="128"/>
+      <c r="I34" s="128"/>
+      <c r="J34" s="129">
+        <v>0</v>
+      </c>
+      <c r="K34" s="126"/>
+    </row>
+    <row r="35" spans="1:11">
+      <c r="A35" s="123" t="s">
+        <v>515</v>
+      </c>
+      <c r="B35" s="124">
+        <v>4</v>
+      </c>
+      <c r="C35" s="123" t="s">
+        <v>421</v>
+      </c>
+      <c r="D35" s="125">
+        <v>495</v>
+      </c>
+      <c r="E35" s="126">
+        <v>0</v>
+      </c>
+      <c r="F35" s="127"/>
+      <c r="G35" s="128"/>
+      <c r="H35" s="128"/>
+      <c r="I35" s="128"/>
+      <c r="J35" s="129">
+        <v>0</v>
+      </c>
+      <c r="K35" s="126"/>
+    </row>
+    <row r="36" spans="1:11">
+      <c r="A36" s="124" t="s">
+        <v>516</v>
+      </c>
+      <c r="B36" s="124">
+        <v>5</v>
+      </c>
+      <c r="C36" s="123" t="s">
+        <v>421</v>
+      </c>
+      <c r="D36" s="125">
+        <v>582</v>
+      </c>
+      <c r="E36" s="126">
+        <v>0</v>
+      </c>
+      <c r="F36" s="127"/>
+      <c r="G36" s="130"/>
+      <c r="H36" s="128" t="s">
+        <v>436</v>
+      </c>
+      <c r="I36" s="128">
+        <v>210</v>
+      </c>
+      <c r="J36" s="129">
+        <v>0</v>
+      </c>
+      <c r="K36" s="126" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11">
+      <c r="A37" s="124" t="s">
+        <v>517</v>
+      </c>
+      <c r="B37" s="124">
+        <v>6</v>
+      </c>
+      <c r="C37" s="123" t="s">
+        <v>421</v>
+      </c>
+      <c r="D37" s="125">
+        <v>561</v>
+      </c>
+      <c r="E37" s="126">
+        <v>10</v>
+      </c>
+      <c r="F37" s="127"/>
+      <c r="G37" s="130"/>
+      <c r="H37" s="128" t="s">
+        <v>436</v>
+      </c>
+      <c r="I37" s="128">
+        <v>240</v>
+      </c>
+      <c r="J37" s="129">
+        <v>0</v>
+      </c>
+      <c r="K37" s="126" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11">
+      <c r="A38" s="124" t="s">
+        <v>518</v>
+      </c>
+      <c r="B38" s="124">
+        <v>6</v>
+      </c>
+      <c r="C38" s="123" t="s">
+        <v>421</v>
+      </c>
+      <c r="D38" s="125">
+        <v>627</v>
+      </c>
+      <c r="E38" s="126">
+        <v>10</v>
+      </c>
+      <c r="F38" s="127"/>
+      <c r="G38" s="130"/>
+      <c r="H38" s="128" t="s">
+        <v>436</v>
+      </c>
+      <c r="I38" s="131">
+        <v>270</v>
+      </c>
+      <c r="J38" s="129">
+        <v>0</v>
+      </c>
+      <c r="K38" s="126" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11">
+      <c r="A39" s="123" t="s">
+        <v>519</v>
+      </c>
+      <c r="B39" s="124">
+        <v>6</v>
+      </c>
+      <c r="C39" s="123" t="s">
+        <v>421</v>
+      </c>
+      <c r="D39" s="125">
+        <v>561</v>
+      </c>
+      <c r="E39" s="126">
+        <v>0</v>
+      </c>
+      <c r="F39" s="127"/>
+      <c r="G39" s="130"/>
+      <c r="H39" s="128" t="s">
+        <v>437</v>
+      </c>
+      <c r="I39" s="128">
+        <v>150</v>
+      </c>
+      <c r="J39" s="129">
+        <v>-10</v>
+      </c>
+      <c r="K39" s="126" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11">
+      <c r="A40" s="123" t="s">
+        <v>520</v>
+      </c>
+      <c r="B40" s="124">
+        <v>8</v>
+      </c>
+      <c r="C40" s="123" t="s">
+        <v>421</v>
+      </c>
+      <c r="D40" s="125">
+        <v>660</v>
+      </c>
+      <c r="E40" s="126">
+        <v>0</v>
+      </c>
+      <c r="F40" s="127"/>
+      <c r="G40" s="130"/>
+      <c r="H40" s="128" t="s">
+        <v>437</v>
+      </c>
+      <c r="I40" s="131">
+        <v>210</v>
+      </c>
+      <c r="J40" s="129">
+        <v>-10</v>
+      </c>
+      <c r="K40" s="126" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11">
+      <c r="A41" s="123" t="s">
+        <v>521</v>
+      </c>
+      <c r="B41" s="124">
+        <v>3</v>
+      </c>
+      <c r="C41" s="123" t="s">
+        <v>421</v>
+      </c>
+      <c r="D41" s="125">
+        <v>462</v>
+      </c>
+      <c r="E41" s="126">
+        <v>0</v>
+      </c>
+      <c r="F41" s="127" t="s">
+        <v>228</v>
+      </c>
+      <c r="G41" s="130">
+        <v>150</v>
+      </c>
+      <c r="H41" s="128"/>
+      <c r="I41" s="128"/>
+      <c r="J41" s="129">
+        <v>-20</v>
+      </c>
+      <c r="K41" s="126"/>
+    </row>
+    <row r="42" spans="1:11">
+      <c r="A42" s="123" t="s">
+        <v>522</v>
+      </c>
+      <c r="B42" s="124">
+        <v>4</v>
+      </c>
+      <c r="C42" s="123" t="s">
+        <v>421</v>
+      </c>
+      <c r="D42" s="125">
+        <v>528</v>
+      </c>
+      <c r="E42" s="126">
+        <v>0</v>
+      </c>
+      <c r="F42" s="127" t="s">
+        <v>228</v>
+      </c>
+      <c r="G42" s="130">
+        <v>210</v>
+      </c>
+      <c r="H42" s="128"/>
+      <c r="I42" s="128"/>
+      <c r="J42" s="129">
+        <v>-20</v>
+      </c>
+      <c r="K42" s="126"/>
+    </row>
+    <row r="43" spans="1:11">
+      <c r="A43" s="123" t="s">
+        <v>523</v>
+      </c>
+      <c r="B43" s="124">
+        <v>5</v>
+      </c>
+      <c r="C43" s="123" t="s">
+        <v>421</v>
+      </c>
+      <c r="D43" s="125">
+        <v>594</v>
+      </c>
+      <c r="E43" s="126">
+        <v>0</v>
+      </c>
+      <c r="F43" s="127" t="s">
+        <v>228</v>
+      </c>
+      <c r="G43" s="130">
+        <v>270</v>
+      </c>
+      <c r="H43" s="128"/>
+      <c r="I43" s="128"/>
+      <c r="J43" s="129">
+        <v>-20</v>
+      </c>
+      <c r="K43" s="126"/>
+    </row>
+    <row r="44" spans="1:11">
+      <c r="A44" s="123" t="s">
+        <v>524</v>
+      </c>
+      <c r="B44" s="124">
+        <v>6</v>
+      </c>
+      <c r="C44" s="123" t="s">
+        <v>421</v>
+      </c>
+      <c r="D44" s="125">
+        <v>660</v>
+      </c>
+      <c r="E44" s="126">
+        <v>0</v>
+      </c>
+      <c r="F44" s="127" t="s">
+        <v>228</v>
+      </c>
+      <c r="G44" s="130">
+        <v>330</v>
+      </c>
+      <c r="H44" s="128"/>
+      <c r="I44" s="128"/>
+      <c r="J44" s="129">
+        <v>-20</v>
+      </c>
+      <c r="K44" s="126"/>
+    </row>
+    <row r="45" spans="1:11">
+      <c r="A45" s="123" t="s">
+        <v>525</v>
+      </c>
+      <c r="B45" s="124">
+        <v>6</v>
+      </c>
+      <c r="C45" s="123" t="s">
+        <v>421</v>
+      </c>
+      <c r="D45" s="125">
+        <v>693</v>
+      </c>
+      <c r="E45" s="126">
+        <v>0</v>
+      </c>
+      <c r="F45" s="127" t="s">
+        <v>228</v>
+      </c>
+      <c r="G45" s="130">
+        <v>390</v>
+      </c>
+      <c r="H45" s="128"/>
+      <c r="I45" s="131"/>
+      <c r="J45" s="129">
+        <v>-20</v>
+      </c>
+      <c r="K45" s="126"/>
+    </row>
+    <row r="46" spans="1:11">
+      <c r="A46" s="123" t="s">
+        <v>526</v>
+      </c>
+      <c r="B46" s="124">
+        <v>2</v>
+      </c>
+      <c r="C46" s="123" t="s">
+        <v>421</v>
+      </c>
+      <c r="D46" s="125">
+        <v>396</v>
+      </c>
+      <c r="E46" s="126">
+        <v>0</v>
+      </c>
+      <c r="F46" s="127" t="s">
+        <v>183</v>
+      </c>
+      <c r="G46" s="130">
+        <v>150</v>
+      </c>
+      <c r="H46" s="128"/>
+      <c r="I46" s="128"/>
+      <c r="J46" s="129">
+        <v>0</v>
+      </c>
+      <c r="K46" s="126"/>
+    </row>
+    <row r="47" spans="1:11">
+      <c r="A47" s="123" t="s">
+        <v>527</v>
+      </c>
+      <c r="B47" s="124">
+        <v>3</v>
+      </c>
+      <c r="C47" s="123" t="s">
+        <v>421</v>
+      </c>
+      <c r="D47" s="125">
+        <v>429</v>
+      </c>
+      <c r="E47" s="126">
+        <v>0</v>
+      </c>
+      <c r="F47" s="127" t="s">
+        <v>183</v>
+      </c>
+      <c r="G47" s="130">
+        <v>180</v>
+      </c>
+      <c r="H47" s="128"/>
+      <c r="I47" s="128"/>
+      <c r="J47" s="129">
+        <v>0</v>
+      </c>
+      <c r="K47" s="126"/>
+    </row>
+    <row r="48" spans="1:11">
+      <c r="A48" s="123" t="s">
+        <v>528</v>
+      </c>
+      <c r="B48" s="124">
+        <v>4</v>
+      </c>
+      <c r="C48" s="123" t="s">
+        <v>421</v>
+      </c>
+      <c r="D48" s="125">
+        <v>462</v>
+      </c>
+      <c r="E48" s="126">
+        <v>0</v>
+      </c>
+      <c r="F48" s="127" t="s">
+        <v>183</v>
+      </c>
+      <c r="G48" s="130">
+        <v>210</v>
+      </c>
+      <c r="H48" s="128"/>
+      <c r="I48" s="128"/>
+      <c r="J48" s="129">
+        <v>0</v>
+      </c>
+      <c r="K48" s="126"/>
+    </row>
+    <row r="49" spans="1:11">
+      <c r="A49" s="123" t="s">
+        <v>529</v>
+      </c>
+      <c r="B49" s="124">
+        <v>5</v>
+      </c>
+      <c r="C49" s="123" t="s">
+        <v>1</v>
+      </c>
+      <c r="D49" s="125">
+        <v>495</v>
+      </c>
+      <c r="E49" s="126">
+        <v>0</v>
+      </c>
+      <c r="F49" s="127" t="s">
+        <v>183</v>
+      </c>
+      <c r="G49" s="130">
+        <v>240</v>
+      </c>
+      <c r="H49" s="128"/>
+      <c r="I49" s="128"/>
+      <c r="J49" s="129">
+        <v>0</v>
+      </c>
+      <c r="K49" s="126" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11">
+      <c r="A50" s="123" t="s">
+        <v>530</v>
+      </c>
+      <c r="B50" s="124">
+        <v>6</v>
+      </c>
+      <c r="C50" s="123" t="s">
+        <v>421</v>
+      </c>
+      <c r="D50" s="125">
+        <v>561</v>
+      </c>
+      <c r="E50" s="126">
+        <v>0</v>
+      </c>
+      <c r="F50" s="127" t="s">
+        <v>183</v>
+      </c>
+      <c r="G50" s="130">
+        <v>300</v>
+      </c>
+      <c r="H50" s="128"/>
+      <c r="I50" s="128"/>
+      <c r="J50" s="129">
+        <v>0</v>
+      </c>
+      <c r="K50" s="126" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11">
+      <c r="A51" s="123" t="s">
+        <v>531</v>
+      </c>
+      <c r="B51" s="124">
+        <v>6</v>
+      </c>
+      <c r="C51" s="123" t="s">
+        <v>421</v>
+      </c>
+      <c r="D51" s="125">
+        <v>627</v>
+      </c>
+      <c r="E51" s="126">
+        <v>0</v>
+      </c>
+      <c r="F51" s="127" t="s">
+        <v>183</v>
+      </c>
+      <c r="G51" s="130">
+        <v>360</v>
+      </c>
+      <c r="H51" s="128"/>
+      <c r="I51" s="131"/>
+      <c r="J51" s="129">
+        <v>0</v>
+      </c>
+      <c r="K51" s="126" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11">
+      <c r="A52" s="123" t="s">
+        <v>532</v>
+      </c>
+      <c r="B52" s="124">
+        <v>7</v>
+      </c>
+      <c r="C52" s="123" t="s">
+        <v>421</v>
+      </c>
+      <c r="D52" s="125">
+        <v>627</v>
+      </c>
+      <c r="E52" s="126">
+        <v>0</v>
+      </c>
+      <c r="F52" s="127" t="s">
+        <v>2</v>
+      </c>
+      <c r="G52" s="130" t="s">
+        <v>533</v>
+      </c>
+      <c r="H52" s="128"/>
+      <c r="I52" s="131"/>
+      <c r="J52" s="129">
+        <v>0</v>
+      </c>
+      <c r="K52" s="126" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11">
+      <c r="A53" s="123" t="s">
+        <v>534</v>
+      </c>
+      <c r="B53" s="124">
+        <v>7</v>
+      </c>
+      <c r="C53" s="123" t="s">
+        <v>421</v>
+      </c>
+      <c r="D53" s="125">
+        <v>660</v>
+      </c>
+      <c r="E53" s="126">
+        <v>0</v>
+      </c>
+      <c r="F53" s="127" t="s">
+        <v>2</v>
+      </c>
+      <c r="G53" s="130" t="s">
+        <v>535</v>
+      </c>
+      <c r="H53" s="128"/>
+      <c r="I53" s="128"/>
+      <c r="J53" s="129">
+        <v>0</v>
+      </c>
+      <c r="K53" s="126" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11">
+      <c r="A54" s="123" t="s">
+        <v>536</v>
+      </c>
+      <c r="B54" s="124">
+        <v>2</v>
+      </c>
+      <c r="C54" s="123" t="s">
+        <v>421</v>
+      </c>
+      <c r="D54" s="125">
+        <v>363</v>
+      </c>
+      <c r="E54" s="126">
+        <v>0</v>
+      </c>
+      <c r="F54" s="127" t="s">
+        <v>27</v>
+      </c>
+      <c r="G54" s="128">
+        <v>120</v>
+      </c>
+      <c r="H54" s="128"/>
+      <c r="I54" s="128"/>
+      <c r="J54" s="129">
+        <v>10</v>
+      </c>
+      <c r="K54" s="126"/>
+    </row>
+    <row r="55" spans="1:11">
+      <c r="A55" s="123" t="s">
+        <v>537</v>
+      </c>
+      <c r="B55" s="124">
+        <v>3</v>
+      </c>
+      <c r="C55" s="123" t="s">
+        <v>421</v>
+      </c>
+      <c r="D55" s="125">
+        <v>396</v>
+      </c>
+      <c r="E55" s="126">
+        <v>0</v>
+      </c>
+      <c r="F55" s="127" t="s">
+        <v>27</v>
+      </c>
+      <c r="G55" s="128">
+        <v>150</v>
+      </c>
+      <c r="H55" s="128"/>
+      <c r="I55" s="128"/>
+      <c r="J55" s="129">
+        <v>10</v>
+      </c>
+      <c r="K55" s="126"/>
+    </row>
+    <row r="56" spans="1:11">
+      <c r="A56" s="123" t="s">
+        <v>538</v>
+      </c>
+      <c r="B56" s="124">
+        <v>4</v>
+      </c>
+      <c r="C56" s="123" t="s">
+        <v>421</v>
+      </c>
+      <c r="D56" s="125">
+        <v>462</v>
+      </c>
+      <c r="E56" s="126">
+        <v>0</v>
+      </c>
+      <c r="F56" s="127" t="s">
+        <v>27</v>
+      </c>
+      <c r="G56" s="128">
+        <v>180</v>
+      </c>
+      <c r="H56" s="128"/>
+      <c r="I56" s="128"/>
+      <c r="J56" s="129">
+        <v>10</v>
+      </c>
+      <c r="K56" s="126"/>
+    </row>
+    <row r="57" spans="1:11">
+      <c r="A57" s="123" t="s">
+        <v>539</v>
+      </c>
+      <c r="B57" s="124">
+        <v>5</v>
+      </c>
+      <c r="C57" s="123" t="s">
+        <v>421</v>
+      </c>
+      <c r="D57" s="125">
+        <v>528</v>
+      </c>
+      <c r="E57" s="126">
+        <v>0</v>
+      </c>
+      <c r="F57" s="127" t="s">
+        <v>27</v>
+      </c>
+      <c r="G57" s="128">
+        <v>210</v>
+      </c>
+      <c r="H57" s="128"/>
+      <c r="I57" s="128"/>
+      <c r="J57" s="129">
+        <v>15</v>
+      </c>
+      <c r="K57" s="126" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11">
+      <c r="A58" s="123" t="s">
+        <v>540</v>
+      </c>
+      <c r="B58" s="124">
+        <v>6</v>
+      </c>
+      <c r="C58" s="123" t="s">
+        <v>421</v>
+      </c>
+      <c r="D58" s="125">
+        <v>561</v>
+      </c>
+      <c r="E58" s="126">
+        <v>0</v>
+      </c>
+      <c r="F58" s="127" t="s">
+        <v>27</v>
+      </c>
+      <c r="G58" s="128">
+        <v>240</v>
+      </c>
+      <c r="H58" s="128"/>
+      <c r="I58" s="128"/>
+      <c r="J58" s="129">
+        <v>15</v>
+      </c>
+      <c r="K58" s="126" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11">
+      <c r="A59" s="123" t="s">
+        <v>541</v>
+      </c>
+      <c r="B59" s="124">
+        <v>6</v>
+      </c>
+      <c r="C59" s="123" t="s">
+        <v>421</v>
+      </c>
+      <c r="D59" s="125">
+        <v>594</v>
+      </c>
+      <c r="E59" s="126">
+        <v>0</v>
+      </c>
+      <c r="F59" s="127" t="s">
+        <v>27</v>
+      </c>
+      <c r="G59" s="128">
+        <v>270</v>
+      </c>
+      <c r="H59" s="128"/>
+      <c r="I59" s="131"/>
+      <c r="J59" s="129">
+        <v>15</v>
+      </c>
+      <c r="K59" s="126" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11">
+      <c r="A60" s="123" t="s">
+        <v>542</v>
+      </c>
+      <c r="B60" s="124">
+        <v>4</v>
+      </c>
+      <c r="C60" s="123" t="s">
+        <v>421</v>
+      </c>
+      <c r="D60" s="125">
+        <v>429</v>
+      </c>
+      <c r="E60" s="126">
+        <v>0</v>
+      </c>
+      <c r="F60" s="127" t="s">
+        <v>69</v>
+      </c>
+      <c r="G60" s="128">
+        <v>210</v>
+      </c>
+      <c r="H60" s="128"/>
+      <c r="I60" s="128"/>
+      <c r="J60" s="129">
+        <v>0</v>
+      </c>
+      <c r="K60" s="126"/>
+    </row>
+    <row r="61" spans="1:11">
+      <c r="A61" s="123" t="s">
+        <v>543</v>
+      </c>
+      <c r="B61" s="124">
+        <v>5</v>
+      </c>
+      <c r="C61" s="123" t="s">
+        <v>421</v>
+      </c>
+      <c r="D61" s="125">
+        <v>462</v>
+      </c>
+      <c r="E61" s="126">
+        <v>0</v>
+      </c>
+      <c r="F61" s="127" t="s">
+        <v>69</v>
+      </c>
+      <c r="G61" s="128">
+        <v>240</v>
+      </c>
+      <c r="H61" s="128"/>
+      <c r="I61" s="128"/>
+      <c r="J61" s="129">
+        <v>0</v>
+      </c>
+      <c r="K61" s="126"/>
+    </row>
+    <row r="62" spans="1:11">
+      <c r="A62" s="123" t="s">
+        <v>544</v>
+      </c>
+      <c r="B62" s="124">
+        <v>6</v>
+      </c>
+      <c r="C62" s="123" t="s">
+        <v>421</v>
+      </c>
+      <c r="D62" s="125">
+        <v>495</v>
+      </c>
+      <c r="E62" s="126">
+        <v>0</v>
+      </c>
+      <c r="F62" s="127" t="s">
+        <v>69</v>
+      </c>
+      <c r="G62" s="128">
+        <v>300</v>
+      </c>
+      <c r="H62" s="128"/>
+      <c r="I62" s="128"/>
+      <c r="J62" s="129">
+        <v>0</v>
+      </c>
+      <c r="K62" s="126"/>
+    </row>
+    <row r="63" spans="1:11">
+      <c r="A63" s="123" t="s">
+        <v>545</v>
+      </c>
+      <c r="B63" s="124">
+        <v>8</v>
+      </c>
+      <c r="C63" s="123" t="s">
+        <v>421</v>
+      </c>
+      <c r="D63" s="125">
+        <v>528</v>
+      </c>
+      <c r="E63" s="126">
+        <v>0</v>
+      </c>
+      <c r="F63" s="127" t="s">
+        <v>69</v>
+      </c>
+      <c r="G63" s="128">
+        <v>360</v>
+      </c>
+      <c r="H63" s="128"/>
+      <c r="I63" s="131"/>
+      <c r="J63" s="129">
+        <v>0</v>
+      </c>
+      <c r="K63" s="126"/>
+    </row>
+    <row r="64" spans="1:11">
+      <c r="A64" s="123" t="s">
+        <v>546</v>
+      </c>
+      <c r="B64" s="124">
+        <v>3</v>
+      </c>
+      <c r="C64" s="123" t="s">
+        <v>421</v>
+      </c>
+      <c r="D64" s="125">
+        <v>396</v>
+      </c>
+      <c r="E64" s="126">
+        <v>0</v>
+      </c>
+      <c r="F64" s="127"/>
+      <c r="G64" s="128"/>
+      <c r="H64" s="128"/>
+      <c r="I64" s="128"/>
+      <c r="J64" s="129">
+        <v>0</v>
+      </c>
+      <c r="K64" s="126"/>
+    </row>
+    <row r="65" spans="1:11">
+      <c r="A65" s="123" t="s">
+        <v>547</v>
+      </c>
+      <c r="B65" s="124">
+        <v>4</v>
+      </c>
+      <c r="C65" s="123" t="s">
+        <v>421</v>
+      </c>
+      <c r="D65" s="125">
+        <v>429</v>
+      </c>
+      <c r="E65" s="126">
+        <v>0</v>
+      </c>
+      <c r="F65" s="127"/>
+      <c r="G65" s="128"/>
+      <c r="H65" s="128"/>
+      <c r="I65" s="128"/>
+      <c r="J65" s="129">
+        <v>0</v>
+      </c>
+      <c r="K65" s="126"/>
+    </row>
+    <row r="66" spans="1:11">
+      <c r="A66" s="123" t="s">
+        <v>548</v>
+      </c>
+      <c r="B66" s="124">
+        <v>5</v>
+      </c>
+      <c r="C66" s="123" t="s">
+        <v>421</v>
+      </c>
+      <c r="D66" s="125">
+        <v>462</v>
+      </c>
+      <c r="E66" s="126">
+        <v>0</v>
+      </c>
+      <c r="F66" s="127"/>
+      <c r="G66" s="128"/>
+      <c r="H66" s="128" t="s">
+        <v>435</v>
+      </c>
+      <c r="I66" s="128">
+        <v>180</v>
+      </c>
+      <c r="J66" s="129">
+        <v>0</v>
+      </c>
+      <c r="K66" s="126" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11">
+      <c r="A67" s="123" t="s">
+        <v>549</v>
+      </c>
+      <c r="B67" s="124">
+        <v>6</v>
+      </c>
+      <c r="C67" s="123" t="s">
+        <v>421</v>
+      </c>
+      <c r="D67" s="125">
+        <v>495</v>
+      </c>
+      <c r="E67" s="126">
+        <v>0</v>
+      </c>
+      <c r="F67" s="127"/>
+      <c r="G67" s="128"/>
+      <c r="H67" s="128" t="s">
+        <v>435</v>
+      </c>
+      <c r="I67" s="128">
+        <v>210</v>
+      </c>
+      <c r="J67" s="129">
+        <v>0</v>
+      </c>
+      <c r="K67" s="126" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="68" spans="1:11">
+      <c r="A68" s="123" t="s">
+        <v>550</v>
+      </c>
+      <c r="B68" s="124">
+        <v>6</v>
+      </c>
+      <c r="C68" s="123" t="s">
+        <v>421</v>
+      </c>
+      <c r="D68" s="125">
+        <v>528</v>
+      </c>
+      <c r="E68" s="126">
+        <v>0</v>
+      </c>
+      <c r="F68" s="127"/>
+      <c r="G68" s="128"/>
+      <c r="H68" s="128" t="s">
+        <v>435</v>
+      </c>
+      <c r="I68" s="131">
+        <v>240</v>
+      </c>
+      <c r="J68" s="129">
+        <v>0</v>
+      </c>
+      <c r="K68" s="126" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="69" spans="1:11">
+      <c r="A69" s="123" t="s">
+        <v>551</v>
+      </c>
+      <c r="B69" s="124">
+        <v>3</v>
+      </c>
+      <c r="C69" s="123" t="s">
+        <v>1</v>
+      </c>
+      <c r="D69" s="125">
+        <v>330</v>
+      </c>
+      <c r="E69" s="126">
+        <v>0</v>
+      </c>
+      <c r="F69" s="127" t="s">
+        <v>2</v>
+      </c>
+      <c r="G69" s="128" t="s">
+        <v>3</v>
+      </c>
+      <c r="H69" s="128"/>
+      <c r="I69" s="128"/>
+      <c r="J69" s="129">
+        <v>0</v>
+      </c>
+      <c r="K69" s="126"/>
+    </row>
+    <row r="70" spans="1:11">
+      <c r="A70" s="123" t="s">
+        <v>552</v>
+      </c>
+      <c r="B70" s="124">
+        <v>4</v>
+      </c>
+      <c r="C70" s="123" t="s">
+        <v>421</v>
+      </c>
+      <c r="D70" s="125">
+        <v>363</v>
+      </c>
+      <c r="E70" s="126">
+        <v>0</v>
+      </c>
+      <c r="F70" s="127" t="s">
+        <v>2</v>
+      </c>
+      <c r="G70" s="128" t="s">
+        <v>12</v>
+      </c>
+      <c r="H70" s="128"/>
+      <c r="I70" s="128"/>
+      <c r="J70" s="129">
+        <v>0</v>
+      </c>
+      <c r="K70" s="126"/>
+    </row>
+    <row r="71" spans="1:11">
+      <c r="A71" s="123" t="s">
+        <v>553</v>
+      </c>
+      <c r="B71" s="124">
+        <v>6</v>
+      </c>
+      <c r="C71" s="123" t="s">
+        <v>421</v>
+      </c>
+      <c r="D71" s="125">
+        <v>528</v>
+      </c>
+      <c r="E71" s="126">
+        <v>0</v>
+      </c>
+      <c r="F71" s="127" t="s">
+        <v>2</v>
+      </c>
+      <c r="G71" s="128" t="s">
+        <v>19</v>
+      </c>
+      <c r="H71" s="128"/>
+      <c r="I71" s="128"/>
+      <c r="J71" s="129">
+        <v>0</v>
+      </c>
+      <c r="K71" s="126" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="72" spans="1:11">
+      <c r="A72" s="123" t="s">
+        <v>554</v>
+      </c>
+      <c r="B72" s="124">
+        <v>5</v>
+      </c>
+      <c r="C72" s="123" t="s">
+        <v>421</v>
+      </c>
+      <c r="D72" s="125">
+        <v>528</v>
+      </c>
+      <c r="E72" s="126">
+        <v>20</v>
+      </c>
+      <c r="F72" s="127"/>
+      <c r="G72" s="128"/>
+      <c r="H72" s="128" t="s">
+        <v>437</v>
+      </c>
+      <c r="I72" s="128">
+        <v>300</v>
+      </c>
+      <c r="J72" s="129">
+        <v>-20</v>
+      </c>
+      <c r="K72" s="126" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="73" spans="1:11">
+      <c r="A73" s="123" t="s">
+        <v>555</v>
+      </c>
+      <c r="B73" s="124">
+        <v>7</v>
+      </c>
+      <c r="C73" s="123" t="s">
+        <v>421</v>
+      </c>
+      <c r="D73" s="125">
+        <v>726</v>
+      </c>
+      <c r="E73" s="126">
+        <v>20</v>
+      </c>
+      <c r="F73" s="127"/>
+      <c r="G73" s="128"/>
+      <c r="H73" s="128" t="s">
+        <v>437</v>
+      </c>
+      <c r="I73" s="128">
+        <v>360</v>
+      </c>
+      <c r="J73" s="129">
+        <v>-20</v>
+      </c>
+      <c r="K73" s="126" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="74" spans="1:11">
+      <c r="A74" s="123" t="s">
+        <v>556</v>
+      </c>
+      <c r="B74" s="124">
+        <v>5</v>
+      </c>
+      <c r="C74" s="123" t="s">
+        <v>1</v>
+      </c>
+      <c r="D74" s="125">
+        <v>330</v>
+      </c>
+      <c r="E74" s="126">
+        <v>0</v>
+      </c>
+      <c r="F74" s="127" t="s">
+        <v>2</v>
+      </c>
+      <c r="G74" s="128" t="s">
+        <v>63</v>
+      </c>
+      <c r="H74" s="128"/>
+      <c r="I74" s="128"/>
+      <c r="J74" s="129">
+        <v>0</v>
+      </c>
+      <c r="K74" s="126"/>
+    </row>
+    <row r="75" spans="1:11">
+      <c r="A75" s="123" t="s">
+        <v>557</v>
+      </c>
+      <c r="B75" s="124">
+        <v>6</v>
+      </c>
+      <c r="C75" s="123" t="s">
+        <v>421</v>
+      </c>
+      <c r="D75" s="125">
+        <v>363</v>
+      </c>
+      <c r="E75" s="126">
+        <v>0</v>
+      </c>
+      <c r="F75" s="127" t="s">
+        <v>2</v>
+      </c>
+      <c r="G75" s="128" t="s">
+        <v>558</v>
+      </c>
+      <c r="H75" s="128"/>
+      <c r="I75" s="128"/>
+      <c r="J75" s="129">
+        <v>0</v>
+      </c>
+      <c r="K75" s="126"/>
+    </row>
+    <row r="76" spans="1:11">
+      <c r="A76" s="123" t="s">
+        <v>559</v>
+      </c>
+      <c r="B76" s="124">
+        <v>7</v>
+      </c>
+      <c r="C76" s="123" t="s">
+        <v>421</v>
+      </c>
+      <c r="D76" s="125">
+        <v>561</v>
+      </c>
+      <c r="E76" s="126">
+        <v>0</v>
+      </c>
+      <c r="F76" s="127"/>
+      <c r="G76" s="128"/>
+      <c r="H76" s="128" t="s">
+        <v>437</v>
+      </c>
+      <c r="I76" s="128">
+        <v>300</v>
+      </c>
+      <c r="J76" s="129">
+        <v>0</v>
+      </c>
+      <c r="K76" s="126"/>
+    </row>
+    <row r="77" spans="1:11">
+      <c r="A77" s="123" t="s">
+        <v>560</v>
+      </c>
+      <c r="B77" s="124">
+        <v>8</v>
+      </c>
+      <c r="C77" s="123" t="s">
+        <v>421</v>
+      </c>
+      <c r="D77" s="125">
+        <v>627</v>
+      </c>
+      <c r="E77" s="126">
+        <v>0</v>
+      </c>
+      <c r="F77" s="127"/>
+      <c r="G77" s="128"/>
+      <c r="H77" s="128" t="s">
+        <v>437</v>
+      </c>
+      <c r="I77" s="128">
+        <v>300</v>
+      </c>
+      <c r="J77" s="129">
+        <v>0</v>
+      </c>
+      <c r="K77" s="126"/>
+    </row>
+    <row r="78" spans="1:11">
+      <c r="A78" s="123" t="s">
+        <v>561</v>
+      </c>
+      <c r="B78" s="124">
+        <v>8</v>
+      </c>
+      <c r="C78" s="123" t="s">
+        <v>421</v>
+      </c>
+      <c r="D78" s="125">
+        <v>594</v>
+      </c>
+      <c r="E78" s="126">
+        <v>0</v>
+      </c>
+      <c r="F78" s="127" t="s">
+        <v>2</v>
+      </c>
+      <c r="G78" s="128" t="s">
+        <v>562</v>
+      </c>
+      <c r="H78" s="128"/>
+      <c r="I78" s="128"/>
+      <c r="J78" s="129">
+        <v>15</v>
+      </c>
+      <c r="K78" s="126" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="79" spans="1:11">
+      <c r="A79" s="123" t="s">
+        <v>563</v>
+      </c>
+      <c r="B79" s="124">
+        <v>6</v>
+      </c>
+      <c r="C79" s="123" t="s">
+        <v>1</v>
+      </c>
+      <c r="D79" s="125">
+        <v>561</v>
+      </c>
+      <c r="E79" s="126">
+        <v>20</v>
+      </c>
+      <c r="F79" s="127" t="s">
+        <v>2</v>
+      </c>
+      <c r="G79" s="128" t="s">
+        <v>489</v>
+      </c>
+      <c r="H79" s="128"/>
+      <c r="I79" s="128"/>
+      <c r="J79" s="129">
+        <v>0</v>
+      </c>
+      <c r="K79" s="126" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="80" spans="1:11">
+      <c r="A80" s="123" t="s">
+        <v>564</v>
+      </c>
+      <c r="B80" s="124">
+        <v>8</v>
+      </c>
+      <c r="C80" s="132" t="s">
+        <v>421</v>
+      </c>
+      <c r="D80" s="125">
+        <v>693</v>
+      </c>
+      <c r="E80" s="126">
+        <v>20</v>
+      </c>
+      <c r="F80" s="127" t="s">
+        <v>2</v>
+      </c>
+      <c r="G80" s="128" t="s">
+        <v>122</v>
+      </c>
+      <c r="H80" s="128"/>
+      <c r="I80" s="128"/>
+      <c r="J80" s="129">
+        <v>0</v>
+      </c>
+      <c r="K80" s="126" t="s">
+        <v>461</v>
+      </c>
+    </row>
+  </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.70" right="0.70" top="0.75" bottom="0.75" header="0.30" footer="0.30"/>
   <pageSetup paperSize="9" orientation="portrait"/>

</xml_diff>